<commit_message>
nuevo nombre del excel
</commit_message>
<xml_diff>
--- a/th.xlsx
+++ b/th.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C1EBF5-C86F-45CC-82F3-85C7E8B07426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBEB23-EBE2-4004-AF97-B13839A4615D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31200" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="238">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t>hola 35</t>
+  </si>
+  <si>
+    <t>hooooola</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EA4913-57E9-4200-BBFB-97C706D3BBD6}">
-  <dimension ref="B1:K106"/>
+  <dimension ref="B1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,6 +2925,11 @@
         <v>236</v>
       </c>
     </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Segundo comiit despues de cambiar el nombre al excel
</commit_message>
<xml_diff>
--- a/th.xlsx
+++ b/th.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBEB23-EBE2-4004-AF97-B13839A4615D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E30EF-AEA8-4822-B53B-56C494C4CD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31200" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="239">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -783,6 +783,9 @@
   </si>
   <si>
     <t>hooooola</t>
+  </si>
+  <si>
+    <t>holaaaaaa2</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EA4913-57E9-4200-BBFB-97C706D3BBD6}">
-  <dimension ref="B1:K110"/>
+  <dimension ref="B1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,6 +2933,11 @@
         <v>237</v>
       </c>
     </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tercer commit despues de cmabiar el nombre a excel
</commit_message>
<xml_diff>
--- a/th.xlsx
+++ b/th.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E30EF-AEA8-4822-B53B-56C494C4CD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB156EC6-1A5C-4A94-9726-E4D61B13E0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31200" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="240">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -786,6 +786,9 @@
   </si>
   <si>
     <t>holaaaaaa2</t>
+  </si>
+  <si>
+    <t>hola 3</t>
   </si>
 </sst>
 </file>
@@ -1212,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EA4913-57E9-4200-BBFB-97C706D3BBD6}">
-  <dimension ref="B1:K111"/>
+  <dimension ref="B1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,6 +2941,11 @@
         <v>238</v>
       </c>
     </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>239</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>